<commit_message>
started coding complex CPU modules
* ALU
* BUS MUX
* CU counter and decoder
* CU logic WIP

also fixed a few ISA bugs
</commit_message>
<xml_diff>
--- a/Firmware/CPU Designs/Complex CPU/ISA and Design.xlsx
+++ b/Firmware/CPU Designs/Complex CPU/ISA and Design.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minec\Desktop\Work\GitHub Repos\PROJ300\Firmware\CPU Designs\Complex CPU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minec\Desktop\github\PROJ300\Firmware\CPU Designs\Complex CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26460626-0AEC-47B6-A7E0-63683602DF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CE8AA6-AE01-4E53-95CE-6BD279DD16DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,15 +51,6 @@
     <t xml:space="preserve">beq(address)              </t>
   </si>
   <si>
-    <t>add(reg, reg/imm, reg/imm)</t>
-  </si>
-  <si>
-    <t>sub(reg, reg/imm, reg/imm)</t>
-  </si>
-  <si>
-    <t>mul(reg, reg/imm, reg/imm)</t>
-  </si>
-  <si>
     <t>no operation</t>
   </si>
   <si>
@@ -162,18 +153,9 @@
     <t>Instruction Code (38-bits)</t>
   </si>
   <si>
-    <t>or(reg, reg/imm, reg/imm)</t>
-  </si>
-  <si>
     <t>1101 s[1..0] a[15..0] b[15..0]</t>
   </si>
   <si>
-    <t>and(reg, reg/imm, reg/imm)</t>
-  </si>
-  <si>
-    <t>mvn(reg, reg/imm)</t>
-  </si>
-  <si>
     <t>reg( a[15..12] ) &lt;- ! b[11..0]</t>
   </si>
   <si>
@@ -225,9 +207,6 @@
     <t>M[b] &lt;- a / reg( a[15..12] )</t>
   </si>
   <si>
-    <t>b - a / reg( a[15..12] )</t>
-  </si>
-  <si>
     <t>top 4 bits of operands 'a' and 'b' is used to select r0-r12; s[1..0] chooses between imm/reg for both operands</t>
   </si>
   <si>
@@ -316,6 +295,27 @@
   </si>
   <si>
     <t>0100 1 s[0] a[15..0] b[15..0]</t>
+  </si>
+  <si>
+    <t>a / reg( a[15..12] ) - b</t>
+  </si>
+  <si>
+    <t>add(reg, imm/reg, imm/reg)</t>
+  </si>
+  <si>
+    <t>sub(reg, imm/reg, imm/reg)</t>
+  </si>
+  <si>
+    <t>mul(reg, imm/reg, imm/reg)</t>
+  </si>
+  <si>
+    <t>and(reg, imm/reg, imm/reg)</t>
+  </si>
+  <si>
+    <t>or(reg, imm/reg, imm/reg)</t>
+  </si>
+  <si>
+    <t>mvn(reg, imm/reg)</t>
   </si>
 </sst>
 </file>
@@ -746,24 +746,24 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.5703125" customWidth="1"/>
-    <col min="4" max="4" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.73046875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.59765625" customWidth="1"/>
+    <col min="4" max="4" width="60.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
@@ -772,434 +772,434 @@
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="2"/>
       <c r="B7" s="8"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
         <v>21</v>
       </c>
-      <c r="E11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="8" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="9"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B24" s="9"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="9"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="9"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="9"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D19" t="s">
+      <c r="B29" s="9"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B30" s="9"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B31" s="9"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="B32" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="9"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="9"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="9"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="9"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="9"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="9"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="9"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="9"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="9"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="14">
         <v>0</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="14">
         <v>1</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="14">
         <v>2</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="14">
         <v>3</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" s="14">
         <v>4</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="14">
         <v>5</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" s="14">
         <v>6</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" s="14">
         <v>7</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="14">
         <v>8</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" s="14">
         <v>9</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" s="14">
         <v>10</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" s="14">
         <v>11</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" s="14">
         <v>12</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B46" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GPR and operand selectors completed
tested as well!
</commit_message>
<xml_diff>
--- a/Firmware/CPU Designs/Complex CPU/ISA and Design.xlsx
+++ b/Firmware/CPU Designs/Complex CPU/ISA and Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minec\Desktop\github\PROJ300\Firmware\CPU Designs\Complex CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CE8AA6-AE01-4E53-95CE-6BD279DD16DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8467E2D1-2A3A-4A03-801F-3C11E888A937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -216,21 +216,6 @@
     <t>reg( a[15..12] ) &lt;- b / reg( b[15..12] )</t>
   </si>
   <si>
-    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[11..8] ) + b[11..0] / reg( b[11..8] )</t>
-  </si>
-  <si>
-    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[11..8] ) - b[11..0] / reg( b[11..8] )</t>
-  </si>
-  <si>
-    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[11..8] ) * b[11..0] / reg( b[11..8] )</t>
-  </si>
-  <si>
-    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[11..8] ) &amp; b[11..0] / reg( b[11..8] )</t>
-  </si>
-  <si>
-    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[11..8] ) | b[11..0] / reg( b[11..8] )</t>
-  </si>
-  <si>
     <t>Generally, the word structure is: OPCODE s[1..0] a[15..0] b[15..0]</t>
   </si>
   <si>
@@ -316,6 +301,21 @@
   </si>
   <si>
     <t>mvn(reg, imm/reg)</t>
+  </si>
+  <si>
+    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[15..12] ) + b[11..0] / reg( b[15..12] )</t>
+  </si>
+  <si>
+    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[15..12] ) - b[11..0] / reg( b[15..12] )</t>
+  </si>
+  <si>
+    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[15..12] ) * b[11..0] / reg( b[15..12] )</t>
+  </si>
+  <si>
+    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[15..12] ) &amp; b[11..0] / reg( b[15..12] )</t>
+  </si>
+  <si>
+    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[15..12] ) | b[11..0] / reg( b[15..12] )</t>
   </si>
 </sst>
 </file>
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -799,7 +799,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>48</v>
@@ -816,7 +816,7 @@
         <v>25</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>49</v>
@@ -833,7 +833,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>50</v>
@@ -855,13 +855,13 @@
         <v>27</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
@@ -943,7 +943,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>54</v>
@@ -952,7 +952,7 @@
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="E14" t="s">
         <v>60</v>
@@ -960,7 +960,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>36</v>
@@ -969,12 +969,12 @@
         <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>37</v>
@@ -983,7 +983,7 @@
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
@@ -991,7 +991,7 @@
         <v>52</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>55</v>
@@ -1005,7 +1005,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>42</v>
@@ -1014,12 +1014,12 @@
         <v>44</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>32</v>
@@ -1028,15 +1028,15 @@
         <v>45</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>46</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B23" s="9"/>
     </row>
@@ -1089,10 +1089,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
@@ -1100,7 +1100,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
@@ -1108,7 +1108,7 @@
         <v>1</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
@@ -1116,7 +1116,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
@@ -1124,7 +1124,7 @@
         <v>3</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
@@ -1132,7 +1132,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
@@ -1140,7 +1140,7 @@
         <v>5</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
@@ -1148,7 +1148,7 @@
         <v>6</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
@@ -1156,7 +1156,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
@@ -1164,7 +1164,7 @@
         <v>8</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.45">
@@ -1172,7 +1172,7 @@
         <v>9</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
@@ -1180,7 +1180,7 @@
         <v>10</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
@@ -1188,7 +1188,7 @@
         <v>11</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
@@ -1196,7 +1196,7 @@
         <v>12</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
preparing CPU for testing
* wired CPU
* started writing instructions in test ROM

** major oversight discovered in AL operations; will work on a compensation mechanism later
</commit_message>
<xml_diff>
--- a/Firmware/CPU Designs/Complex CPU/ISA and Design.xlsx
+++ b/Firmware/CPU Designs/Complex CPU/ISA and Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minec\Desktop\github\PROJ300\Firmware\CPU Designs\Complex CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8467E2D1-2A3A-4A03-801F-3C11E888A937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968E041F-C817-4C93-A9B3-96F402FDC2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,9 +105,6 @@
     <t xml:space="preserve">ldr(reg, address/value)   </t>
   </si>
   <si>
-    <t xml:space="preserve">str(imm/reg, address in mem)   </t>
-  </si>
-  <si>
     <t xml:space="preserve">cmp(reg, imm/reg)     </t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>1101 s[1..0] a[15..0] b[15..0]</t>
   </si>
   <si>
-    <t>reg( a[15..12] ) &lt;- ! b[11..0]</t>
-  </si>
-  <si>
     <t>logical and</t>
   </si>
   <si>
@@ -195,9 +189,6 @@
     <t>logical shift to right (div by 2^n)</t>
   </si>
   <si>
-    <t>reg( a[15..12] ) &lt;- reg( a[15..12] ) &gt;&gt; b</t>
-  </si>
-  <si>
     <t>s is don't care</t>
   </si>
   <si>
@@ -303,19 +294,28 @@
     <t>mvn(reg, imm/reg)</t>
   </si>
   <si>
-    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[15..12] ) + b[11..0] / reg( b[15..12] )</t>
-  </si>
-  <si>
-    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[15..12] ) - b[11..0] / reg( b[15..12] )</t>
-  </si>
-  <si>
-    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[15..12] ) * b[11..0] / reg( b[15..12] )</t>
-  </si>
-  <si>
-    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[15..12] ) &amp; b[11..0] / reg( b[15..12] )</t>
-  </si>
-  <si>
-    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[15..12] ) | b[11..0] / reg( b[15..12] )</t>
+    <t xml:space="preserve">str(reg/imm, address in mem)   </t>
+  </si>
+  <si>
+    <t>reg( a[11..8] ) &lt;- a[11..0] / reg( a[15..12] ) + b[11..0] / reg( b[15..12] )</t>
+  </si>
+  <si>
+    <t>reg( a[11..8] ) &lt;- a[11..0] / reg( a[15..12] ) - b[11..0] / reg( b[15..12] )</t>
+  </si>
+  <si>
+    <t>reg( a[11..8] ) &lt;- a[11..0] / reg( a[15..12] ) * b[11..0] / reg( b[15..12] )</t>
+  </si>
+  <si>
+    <t>reg( a[11..8] ) &lt;- reg( a[15..12] ) &gt;&gt; b</t>
+  </si>
+  <si>
+    <t>reg( a[11..8] ) &lt;- a[11..0] / reg( a[15..12] ) &amp; b[11..0] / reg( b[15..12] )</t>
+  </si>
+  <si>
+    <t>reg( a[11..8] ) &lt;- a[11..0] / reg( a[15..12] ) | b[11..0] / reg( b[15..12] )</t>
+  </si>
+  <si>
+    <t>reg( a[11..8] ) &lt;- ! b[11..0]</t>
   </si>
 </sst>
 </file>
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -760,10 +760,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
@@ -780,7 +780,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>8</v>
@@ -799,16 +799,16 @@
         <v>24</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -816,33 +816,33 @@
         <v>25</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -852,19 +852,19 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
@@ -872,7 +872,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>9</v>
@@ -886,7 +886,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>10</v>
@@ -903,7 +903,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>11</v>
@@ -920,7 +920,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>12</v>
@@ -943,111 +943,111 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="D18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B23" s="9"/>
     </row>
@@ -1062,13 +1062,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="9"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" s="9"/>
     </row>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B29" s="9"/>
     </row>
@@ -1089,10 +1089,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
@@ -1100,7 +1100,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
@@ -1108,7 +1108,7 @@
         <v>1</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
@@ -1116,7 +1116,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
@@ -1124,7 +1124,7 @@
         <v>3</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
@@ -1132,7 +1132,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
@@ -1140,7 +1140,7 @@
         <v>5</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
@@ -1148,7 +1148,7 @@
         <v>6</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
@@ -1156,7 +1156,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
@@ -1164,7 +1164,7 @@
         <v>8</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.45">
@@ -1172,7 +1172,7 @@
         <v>9</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
@@ -1180,7 +1180,7 @@
         <v>10</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
@@ -1188,7 +1188,7 @@
         <v>11</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
@@ -1196,7 +1196,7 @@
         <v>12</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
[UNTESTED] finished wiring CPU
* compensated for ALU oversight spoken about in previous commit
* filled test ROM will all possible instruction combinations ready for testing
* fixed bugs causing some components to not infer purely combinational logic
* added comments

* will test later...
</commit_message>
<xml_diff>
--- a/Firmware/CPU Designs/Complex CPU/ISA and Design.xlsx
+++ b/Firmware/CPU Designs/Complex CPU/ISA and Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minec\Desktop\github\PROJ300\Firmware\CPU Designs\Complex CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968E041F-C817-4C93-A9B3-96F402FDC2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E3DBEA-8A7C-47BD-A1C2-9B86D45D60D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -297,25 +297,25 @@
     <t xml:space="preserve">str(reg/imm, address in mem)   </t>
   </si>
   <si>
-    <t>reg( a[11..8] ) &lt;- a[11..0] / reg( a[15..12] ) + b[11..0] / reg( b[15..12] )</t>
-  </si>
-  <si>
-    <t>reg( a[11..8] ) &lt;- a[11..0] / reg( a[15..12] ) - b[11..0] / reg( b[15..12] )</t>
-  </si>
-  <si>
-    <t>reg( a[11..8] ) &lt;- a[11..0] / reg( a[15..12] ) * b[11..0] / reg( b[15..12] )</t>
-  </si>
-  <si>
-    <t>reg( a[11..8] ) &lt;- reg( a[15..12] ) &gt;&gt; b</t>
-  </si>
-  <si>
-    <t>reg( a[11..8] ) &lt;- a[11..0] / reg( a[15..12] ) &amp; b[11..0] / reg( b[15..12] )</t>
-  </si>
-  <si>
-    <t>reg( a[11..8] ) &lt;- a[11..0] / reg( a[15..12] ) | b[11..0] / reg( b[15..12] )</t>
-  </si>
-  <si>
-    <t>reg( a[11..8] ) &lt;- ! b[11..0]</t>
+    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[11..8] ) + b[11..0] / reg( b[11..8] )</t>
+  </si>
+  <si>
+    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[11..8] ) - b[11..0] / reg( b[11..8] )</t>
+  </si>
+  <si>
+    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[11..8] ) * b[11..0] / reg( b[11..8] )</t>
+  </si>
+  <si>
+    <t>reg( a[15..12] ) &lt;- reg( a[11..8] ) &gt;&gt; b</t>
+  </si>
+  <si>
+    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[11..8] ) | b[11..0] / reg( b[11..8] )</t>
+  </si>
+  <si>
+    <t>reg( a[15..12] ) &lt;- a[11..0] / reg( a[11..8] ) &amp; b[11..0] / reg( b[11..8] )</t>
+  </si>
+  <si>
+    <t>reg( a[15..12] ) &lt;- ! b[11..0] / !reg( b[15..12] )</t>
   </si>
 </sst>
 </file>
@@ -746,7 +746,7 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1014,7 +1014,7 @@
         <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1028,7 +1028,7 @@
         <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">

</xml_diff>